<commit_message>
GenTable updates and URS Updates: L2/L8
</commit_message>
<xml_diff>
--- a/DbLayouts/L1-顧客管理作業/CustMain.xlsx
+++ b/DbLayouts/L1-顧客管理作業/CustMain.xlsx
@@ -15,7 +15,7 @@
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
     <sheet name="DBS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -601,10 +601,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>開放查詢</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>共用代碼檔
 1:小學以下
 2:國中
@@ -901,6 +897,10 @@
   </si>
   <si>
     <t>CuscCd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>開放查詢</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1487,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1511,7 +1511,7 @@
         <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="11"/>
@@ -1521,7 +1521,7 @@
       <c r="A2" s="31"/>
       <c r="B2" s="32"/>
       <c r="C2" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>66</v>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="B3" s="32"/>
       <c r="C3" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>82</v>
@@ -1625,10 +1625,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>10</v>
@@ -1645,10 +1645,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>10</v>
@@ -1668,7 +1668,7 @@
         <v>83</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>100</v>
@@ -1687,7 +1687,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>18</v>
@@ -1782,7 +1782,7 @@
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -1791,7 +1791,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>7</v>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -1813,10 +1813,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>10</v>
@@ -1835,10 +1835,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>10</v>
@@ -1848,7 +1848,7 @@
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -1900,7 +1900,7 @@
         <v>85</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>10</v>
@@ -1920,7 +1920,7 @@
         <v>86</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>10</v>
@@ -1940,7 +1940,7 @@
         <v>87</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>10</v>
@@ -1962,7 +1962,7 @@
         <v>88</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>10</v>
@@ -2164,7 +2164,7 @@
         <v>104</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>10</v>
@@ -2385,20 +2385,20 @@
         <v>38</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E46" s="25">
         <v>1</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
@@ -2410,7 +2410,7 @@
         <v>96</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>10</v>
@@ -2420,7 +2420,7 @@
       </c>
       <c r="F47" s="18"/>
       <c r="G47" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="1" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
@@ -2451,7 +2451,7 @@
         <v>41</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C49" s="24" t="s">
         <v>42</v>
@@ -2484,7 +2484,7 @@
       </c>
       <c r="F50" s="24"/>
       <c r="G50" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="1" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
@@ -2638,7 +2638,7 @@
         <v>54</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D58" s="24" t="s">
         <v>10</v>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="F58" s="24"/>
       <c r="G58" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2757,10 +2757,10 @@
         <v>56</v>
       </c>
       <c r="B64" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64" s="24" t="s">
         <v>146</v>
-      </c>
-      <c r="C64" s="24" t="s">
-        <v>147</v>
       </c>
       <c r="D64" s="24" t="s">
         <v>100</v>
@@ -2777,13 +2777,13 @@
         <v>57</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>144</v>
+        <v>212</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E65" s="24">
         <v>1</v>
@@ -2797,10 +2797,10 @@
         <v>58</v>
       </c>
       <c r="B66" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C66" s="18" t="s">
         <v>151</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>152</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>10</v>
@@ -2817,10 +2817,10 @@
         <v>59</v>
       </c>
       <c r="B67" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C67" s="20" t="s">
         <v>154</v>
-      </c>
-      <c r="C67" s="20" t="s">
-        <v>155</v>
       </c>
       <c r="D67" s="23" t="s">
         <v>72</v>
@@ -2830,7 +2830,7 @@
       </c>
       <c r="F67" s="21"/>
       <c r="G67" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -2839,10 +2839,10 @@
         <v>60</v>
       </c>
       <c r="B68" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>10</v>
@@ -2852,7 +2852,7 @@
       </c>
       <c r="F68" s="29"/>
       <c r="G68" s="28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
@@ -2861,10 +2861,10 @@
         <v>61</v>
       </c>
       <c r="B69" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D69" s="25" t="s">
         <v>10</v>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="F69" s="29"/>
       <c r="G69" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
@@ -2883,10 +2883,10 @@
         <v>62</v>
       </c>
       <c r="B70" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D70" s="25" t="s">
         <v>10</v>
@@ -2896,7 +2896,7 @@
       </c>
       <c r="F70" s="29"/>
       <c r="G70" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
@@ -2905,10 +2905,10 @@
         <v>63</v>
       </c>
       <c r="B71" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D71" s="25" t="s">
         <v>10</v>
@@ -2918,7 +2918,7 @@
       </c>
       <c r="F71" s="29"/>
       <c r="G71" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -2927,20 +2927,20 @@
         <v>64</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E72" s="25">
         <v>1</v>
       </c>
       <c r="F72" s="29"/>
       <c r="G72" s="28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="81" x14ac:dyDescent="0.3">
@@ -2949,10 +2949,10 @@
         <v>65</v>
       </c>
       <c r="B73" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D73" s="25" t="s">
         <v>100</v>
@@ -2962,7 +2962,7 @@
       </c>
       <c r="F73" s="29"/>
       <c r="G73" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -3043,7 +3043,7 @@
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D84" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.3">
@@ -3101,10 +3101,10 @@
         <v>64</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3117,24 +3117,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>136</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3153,7 +3153,7 @@
         <v>80</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -3177,13 +3177,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Multiple URS Updates; GenTable updates
L1, L3; Replies to SKL inquiries
</commit_message>
<xml_diff>
--- a/DbLayouts/L1-顧客管理作業/CustMain.xlsx
+++ b/DbLayouts/L1-顧客管理作業/CustMain.xlsx
@@ -15,7 +15,7 @@
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
     <sheet name="DBS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -256,9 +256,6 @@
     <t>年收入</t>
   </si>
   <si>
-    <t>IncomeDataDate</t>
-  </si>
-  <si>
     <t>護照號碼</t>
   </si>
   <si>
@@ -676,10 +673,6 @@
   </si>
   <si>
     <t>介紹人</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Introducer</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -906,6 +899,14 @@
   <si>
     <t>1:不開放 
 2:開放</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Introducer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IncomeDataDate</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1492,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1509,14 +1510,14 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="11"/>
@@ -1526,10 +1527,10 @@
       <c r="A2" s="31"/>
       <c r="B2" s="32"/>
       <c r="C2" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -1537,14 +1538,14 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="32"/>
       <c r="C3" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
@@ -1563,14 +1564,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="32"/>
       <c r="C5" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>81</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>82</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -1578,11 +1579,11 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="32"/>
       <c r="C6" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="14"/>
@@ -1591,11 +1592,11 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="32"/>
       <c r="C7" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="14"/>
@@ -1604,7 +1605,7 @@
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>12</v>
@@ -1630,10 +1631,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>10</v>
@@ -1650,10 +1651,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>10</v>
@@ -1670,20 +1671,20 @@
         <v>3</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E11" s="18">
         <v>7</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1692,7 +1693,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>18</v>
@@ -1712,7 +1713,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>3</v>
@@ -1738,7 +1739,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E14" s="18">
         <v>8</v>
@@ -1752,7 +1753,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>5</v>
@@ -1765,7 +1766,7 @@
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="162" x14ac:dyDescent="0.3">
@@ -1774,7 +1775,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>6</v>
@@ -1787,7 +1788,7 @@
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -1796,7 +1797,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>7</v>
@@ -1809,7 +1810,7 @@
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -1818,10 +1819,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>10</v>
@@ -1831,7 +1832,7 @@
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
@@ -1840,10 +1841,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>192</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>194</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>10</v>
@@ -1853,7 +1854,7 @@
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -1865,7 +1866,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>10</v>
@@ -1902,10 +1903,10 @@
         <v>14</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>10</v>
@@ -1922,10 +1923,10 @@
         <v>15</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>10</v>
@@ -1942,10 +1943,10 @@
         <v>16</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>10</v>
@@ -1955,7 +1956,7 @@
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1964,10 +1965,10 @@
         <v>17</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>10</v>
@@ -1977,7 +1978,7 @@
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1986,7 +1987,7 @@
         <v>18</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>23</v>
@@ -2006,7 +2007,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>24</v>
@@ -2026,7 +2027,7 @@
         <v>20</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>25</v>
@@ -2046,7 +2047,7 @@
         <v>21</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>26</v>
@@ -2066,7 +2067,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>27</v>
@@ -2086,7 +2087,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>28</v>
@@ -2106,7 +2107,7 @@
         <v>24</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>29</v>
@@ -2126,7 +2127,7 @@
         <v>25</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>30</v>
@@ -2146,7 +2147,7 @@
         <v>26</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>31</v>
@@ -2166,10 +2167,10 @@
         <v>27</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>10</v>
@@ -2186,7 +2187,7 @@
         <v>28</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>32</v>
@@ -2199,7 +2200,7 @@
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2208,7 +2209,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>33</v>
@@ -2221,7 +2222,7 @@
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2230,7 +2231,7 @@
         <v>30</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>34</v>
@@ -2250,7 +2251,7 @@
         <v>31</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>35</v>
@@ -2270,7 +2271,7 @@
         <v>32</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>36</v>
@@ -2290,7 +2291,7 @@
         <v>33</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>37</v>
@@ -2310,7 +2311,7 @@
         <v>34</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>38</v>
@@ -2330,7 +2331,7 @@
         <v>35</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>39</v>
@@ -2350,7 +2351,7 @@
         <v>36</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>40</v>
@@ -2370,7 +2371,7 @@
         <v>37</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>41</v>
@@ -2390,20 +2391,20 @@
         <v>38</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C46" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="D46" s="25" t="s">
         <v>208</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>210</v>
       </c>
       <c r="E46" s="25">
         <v>1</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
@@ -2412,10 +2413,10 @@
         <v>39</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>10</v>
@@ -2425,7 +2426,7 @@
       </c>
       <c r="F47" s="18"/>
       <c r="G47" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="1" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
@@ -2434,7 +2435,7 @@
         <v>40</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C48" s="24" t="s">
         <v>9</v>
@@ -2447,7 +2448,7 @@
       </c>
       <c r="F48" s="24"/>
       <c r="G48" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2456,7 +2457,7 @@
         <v>41</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C49" s="24" t="s">
         <v>42</v>
@@ -2476,7 +2477,7 @@
         <v>42</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C50" s="24" t="s">
         <v>43</v>
@@ -2489,7 +2490,7 @@
       </c>
       <c r="F50" s="24"/>
       <c r="G50" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="1" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
@@ -2498,7 +2499,7 @@
         <v>43</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C51" s="24" t="s">
         <v>44</v>
@@ -2511,7 +2512,7 @@
       </c>
       <c r="F51" s="24"/>
       <c r="G51" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2520,7 +2521,7 @@
         <v>44</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C52" s="24" t="s">
         <v>45</v>
@@ -2540,7 +2541,7 @@
         <v>45</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C53" s="24" t="s">
         <v>46</v>
@@ -2560,7 +2561,7 @@
         <v>46</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C54" s="24" t="s">
         <v>47</v>
@@ -2626,7 +2627,7 @@
         <v>53</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E57" s="24">
         <v>9</v>
@@ -2640,10 +2641,10 @@
         <v>50</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>54</v>
+        <v>213</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D58" s="24" t="s">
         <v>10</v>
@@ -2653,7 +2654,7 @@
       </c>
       <c r="F58" s="24"/>
       <c r="G58" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2662,10 +2663,10 @@
         <v>51</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D59" s="24" t="s">
         <v>10</v>
@@ -2682,10 +2683,10 @@
         <v>52</v>
       </c>
       <c r="B60" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" s="24" t="s">
         <v>56</v>
-      </c>
-      <c r="C60" s="24" t="s">
-        <v>57</v>
       </c>
       <c r="D60" s="24" t="s">
         <v>10</v>
@@ -2702,10 +2703,10 @@
         <v>53</v>
       </c>
       <c r="B61" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C61" s="24" t="s">
         <v>58</v>
-      </c>
-      <c r="C61" s="24" t="s">
-        <v>59</v>
       </c>
       <c r="D61" s="24" t="s">
         <v>10</v>
@@ -2722,10 +2723,10 @@
         <v>54</v>
       </c>
       <c r="B62" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="18" t="s">
         <v>60</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>61</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>19</v>
@@ -2742,13 +2743,13 @@
         <v>55</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D63" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E63" s="24">
         <v>3</v>
@@ -2762,13 +2763,13 @@
         <v>56</v>
       </c>
       <c r="B64" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C64" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="C64" s="24" t="s">
-        <v>146</v>
-      </c>
       <c r="D64" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E64" s="24">
         <v>3</v>
@@ -2782,20 +2783,20 @@
         <v>57</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E65" s="24">
         <v>1</v>
       </c>
       <c r="F65" s="24"/>
       <c r="G65" s="24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2804,10 +2805,10 @@
         <v>58</v>
       </c>
       <c r="B66" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C66" s="18" t="s">
         <v>150</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>151</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>10</v>
@@ -2824,20 +2825,20 @@
         <v>59</v>
       </c>
       <c r="B67" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C67" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="C67" s="20" t="s">
-        <v>154</v>
-      </c>
       <c r="D67" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E67" s="23">
         <v>1</v>
       </c>
       <c r="F67" s="21"/>
       <c r="G67" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -2846,10 +2847,10 @@
         <v>60</v>
       </c>
       <c r="B68" s="27" t="s">
-        <v>162</v>
+        <v>212</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>10</v>
@@ -2859,7 +2860,7 @@
       </c>
       <c r="F68" s="29"/>
       <c r="G68" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
@@ -2868,10 +2869,10 @@
         <v>61</v>
       </c>
       <c r="B69" s="27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D69" s="25" t="s">
         <v>10</v>
@@ -2881,7 +2882,7 @@
       </c>
       <c r="F69" s="29"/>
       <c r="G69" s="28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
@@ -2890,10 +2891,10 @@
         <v>62</v>
       </c>
       <c r="B70" s="27" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D70" s="25" t="s">
         <v>10</v>
@@ -2903,7 +2904,7 @@
       </c>
       <c r="F70" s="29"/>
       <c r="G70" s="28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
@@ -2912,10 +2913,10 @@
         <v>63</v>
       </c>
       <c r="B71" s="27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D71" s="25" t="s">
         <v>10</v>
@@ -2925,7 +2926,7 @@
       </c>
       <c r="F71" s="29"/>
       <c r="G71" s="28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -2934,20 +2935,20 @@
         <v>64</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E72" s="25">
         <v>1</v>
       </c>
       <c r="F72" s="29"/>
       <c r="G72" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="81" x14ac:dyDescent="0.3">
@@ -2956,20 +2957,20 @@
         <v>65</v>
       </c>
       <c r="B73" s="27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D73" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E73" s="30">
         <v>1</v>
       </c>
       <c r="F73" s="29"/>
       <c r="G73" s="28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -2978,13 +2979,13 @@
         <v>66</v>
       </c>
       <c r="B74" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D74" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="C74" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D74" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="E74" s="18"/>
       <c r="F74" s="18"/>
@@ -2996,10 +2997,10 @@
         <v>67</v>
       </c>
       <c r="B75" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C75" s="18" t="s">
         <v>74</v>
-      </c>
-      <c r="C75" s="18" t="s">
-        <v>75</v>
       </c>
       <c r="D75" s="18" t="s">
         <v>10</v>
@@ -3016,13 +3017,13 @@
         <v>68</v>
       </c>
       <c r="B76" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C76" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C76" s="18" t="s">
-        <v>77</v>
-      </c>
       <c r="D76" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E76" s="18"/>
       <c r="F76" s="18"/>
@@ -3033,10 +3034,10 @@
         <v>69</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D77" s="18" t="s">
         <v>10</v>
@@ -3050,7 +3051,7 @@
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D84" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.3">
@@ -3105,92 +3106,92 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>